<commit_message>
adding combining years script
</commit_message>
<xml_diff>
--- a/Metagenomic_assembly_analysis/tables/functional_difabund.xlsx
+++ b/Metagenomic_assembly_analysis/tables/functional_difabund.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/elizabethmallott/Dropbox/Projects/VMI/vmi_hmp/VMI-diet-challenge/Metagenomic_assembly_analysis/tables/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1AB8209B-94BE-7D4A-AEAF-7EEA80104B88}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{86EB3320-0576-BA4F-87C4-C5A14C193ED8}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2100" yWindow="500" windowWidth="23900" windowHeight="17260" activeTab="5" xr2:uid="{043AAEB4-E59E-194D-90D5-AD8CE91D0B53}"/>
+    <workbookView xWindow="-24260" yWindow="2580" windowWidth="23900" windowHeight="17260" activeTab="5" xr2:uid="{043AAEB4-E59E-194D-90D5-AD8CE91D0B53}"/>
   </bookViews>
   <sheets>
     <sheet name="cog_fecal" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">cog_fecal!$A$1:$F$121</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">cog_oral!$A$1:$F$121</definedName>
   </definedNames>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -323,7 +323,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -334,6 +334,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="11" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -651,7 +652,7 @@
   <dimension ref="A1:G123"/>
   <sheetViews>
     <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2073,7 +2074,7 @@
   <dimension ref="A1:F121"/>
   <sheetViews>
     <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2:F25"/>
+      <selection activeCell="C2" sqref="C2:C25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2641,7 +2642,7 @@
   <dimension ref="A1:F22"/>
   <sheetViews>
     <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="D19" sqref="D19"/>
+      <selection activeCell="D2" sqref="D2:D21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4083,15 +4084,15 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{32FE6696-C653-E348-8425-A9BAA92D6A0A}">
-  <dimension ref="A1:G26"/>
+  <dimension ref="A1:H26"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="G27" sqref="G27"/>
+      <selection activeCell="H3" sqref="H3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -4111,7 +4112,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>49</v>
       </c>
@@ -4130,8 +4131,9 @@
       <c r="F2">
         <v>1.780605E-2</v>
       </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H2" s="10"/>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
         <v>50</v>
       </c>
@@ -4154,7 +4156,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
         <v>51</v>
       </c>
@@ -4177,7 +4179,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
         <v>52</v>
       </c>
@@ -4200,7 +4202,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
         <v>53</v>
       </c>
@@ -4223,7 +4225,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A7" s="2" t="s">
         <v>54</v>
       </c>
@@ -4246,7 +4248,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A8" s="2" t="s">
         <v>55</v>
       </c>
@@ -4269,7 +4271,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A9" s="2" t="s">
         <v>56</v>
       </c>
@@ -4292,7 +4294,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>57</v>
       </c>
@@ -4312,7 +4314,7 @@
         <v>2.0035769999999999E-3</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A11" s="2" t="s">
         <v>58</v>
       </c>
@@ -4335,7 +4337,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>59</v>
       </c>
@@ -4355,7 +4357,7 @@
         <v>1.56986E-3</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A13" s="2" t="s">
         <v>60</v>
       </c>
@@ -4378,7 +4380,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A14" s="2" t="s">
         <v>61</v>
       </c>
@@ -4401,7 +4403,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A15" s="2" t="s">
         <v>62</v>
       </c>
@@ -4424,7 +4426,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A16" s="2" t="s">
         <v>63</v>
       </c>

</xml_diff>